<commit_message>
Status code fixed and minor bug solved
</commit_message>
<xml_diff>
--- a/invoices/sales_report.xlsx
+++ b/invoices/sales_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>SL No</t>
   </si>
@@ -43,12 +43,33 @@
     <t>Status</t>
   </si>
   <si>
+    <t>#FBZ-L1V4H3K</t>
+  </si>
+  <si>
+    <t>Joyal Kuriakose</t>
+  </si>
+  <si>
+    <t>2025-02-04</t>
+  </si>
+  <si>
+    <t>Holistic Fitness 6kg Rubber Slam Ball</t>
+  </si>
+  <si>
+    <t>4,599</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>netbanking</t>
+  </si>
+  <si>
+    <t>Shipped</t>
+  </si>
+  <si>
     <t>#FBZ-L1RGCSK</t>
   </si>
   <si>
-    <t>Joyal Kuriakose</t>
-  </si>
-  <si>
     <t>2025-01-04</t>
   </si>
   <si>
@@ -58,60 +79,39 @@
     <t>829</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>netbanking</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>#FBZ-L1V4H3K</t>
-  </si>
-  <si>
-    <t>2025-02-04</t>
-  </si>
-  <si>
-    <t>Holistic Fitness 6kg Rubber Slam Ball</t>
-  </si>
-  <si>
-    <t>4,599</t>
-  </si>
-  <si>
-    <t>Shipped</t>
+    <t>#FBZ-6C73256</t>
+  </si>
+  <si>
+    <t>Joyal K</t>
+  </si>
+  <si>
+    <t>2025-04-04</t>
+  </si>
+  <si>
+    <t>4,539</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>Delivered</t>
   </si>
   <si>
     <t>#FBZ-6C4S67Y</t>
   </si>
   <si>
-    <t>Joyal K</t>
-  </si>
-  <si>
     <t>2025-03-04</t>
   </si>
   <si>
     <t>769</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>cod</t>
-  </si>
-  <si>
-    <t>#FBZ-6C73256</t>
-  </si>
-  <si>
-    <t>2025-04-04</t>
-  </si>
-  <si>
-    <t>4,539</t>
-  </si>
-  <si>
-    <t>Delivered</t>
-  </si>
-  <si>
     <t>#FBZ-QC1Q4GX</t>
   </si>
   <si>
@@ -169,6 +169,21 @@
     <t>300</t>
   </si>
   <si>
+    <t>#FBZ-328BOQA</t>
+  </si>
+  <si>
+    <t>Achu K</t>
+  </si>
+  <si>
+    <t>2025-04-06</t>
+  </si>
+  <si>
+    <t>629</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
     <t>Summary:</t>
   </si>
   <si>
@@ -181,19 +196,19 @@
     <t>Total Amount (₹)</t>
   </si>
   <si>
-    <t>₹27,496</t>
+    <t>₹28,125</t>
   </si>
   <si>
     <t>Total Discounts (₹)</t>
   </si>
   <si>
-    <t>₹540</t>
+    <t>₹740</t>
   </si>
   <si>
     <t>Net Sales (₹)</t>
   </si>
   <si>
-    <t>₹26,956</t>
+    <t>₹27,385</t>
   </si>
 </sst>
 </file>
@@ -570,7 +585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -709,7 +724,7 @@
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -717,13 +732,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -732,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
         <v>27</v>
@@ -741,7 +756,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -755,7 +770,7 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>35</v>
@@ -773,7 +788,7 @@
         <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -787,7 +802,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>38</v>
@@ -805,7 +820,7 @@
         <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -851,7 +866,7 @@
         <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>49</v>
@@ -869,51 +884,83 @@
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C10" t="s">
         <v>53</v>
       </c>
-      <c r="G11">
-        <v>8</v>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="G14" t="s">
-        <v>60</v>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
partialy done transaction management
</commit_message>
<xml_diff>
--- a/invoices/sales_report.xlsx
+++ b/invoices/sales_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
   <si>
     <t>SL No</t>
   </si>
@@ -43,145 +43,157 @@
     <t>Status</t>
   </si>
   <si>
-    <t>#FBZ-L1V4H3K</t>
+    <t>#FBZ-115EG1Y</t>
+  </si>
+  <si>
+    <t>Joyal K</t>
+  </si>
+  <si>
+    <t>2025-04-06</t>
+  </si>
+  <si>
+    <t>Kettle Bell 6 Kgs for home gym</t>
+  </si>
+  <si>
+    <t>1,008</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>netbanking</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>#FBZ-117E3WP</t>
+  </si>
+  <si>
+    <t>2025-04-05</t>
+  </si>
+  <si>
+    <t>Sports Premium Blitz Blue Kettlebell 8kg Cast Iron Vinyl Coated Solid Kettlebell</t>
+  </si>
+  <si>
+    <t>1,635</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>#FBZ-PBMIZYX</t>
+  </si>
+  <si>
+    <t>Abhinav K</t>
+  </si>
+  <si>
+    <t>2025-04-04</t>
+  </si>
+  <si>
+    <t>Cast Iron Vinyl Coated Dumbbells for gym Workout</t>
+  </si>
+  <si>
+    <t>599</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>wallet</t>
+  </si>
+  <si>
+    <t>#FBZ-TM3CGR9</t>
+  </si>
+  <si>
+    <t>Cezanne P</t>
+  </si>
+  <si>
+    <t>2025-04-03</t>
+  </si>
+  <si>
+    <t>MEDIX Soft Medicine Ball (2), Rubber for Adults</t>
+  </si>
+  <si>
+    <t>629</t>
+  </si>
+  <si>
+    <t>#FBZ-VDGHF7G</t>
+  </si>
+  <si>
+    <t>Achyuth J</t>
+  </si>
+  <si>
+    <t>2025-04-02</t>
+  </si>
+  <si>
+    <t>Rubber Medicine Ball Weights for men &amp; women</t>
+  </si>
+  <si>
+    <t>2,052</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>#FBZ-XIPA8OQ</t>
+  </si>
+  <si>
+    <t>Achu K</t>
+  </si>
+  <si>
+    <t>2025-04-01</t>
+  </si>
+  <si>
+    <t>Pair of two PVC Dumbbells Set Hex for all</t>
+  </si>
+  <si>
+    <t>1,065</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>#FBZ-9VZ5PY4</t>
+  </si>
+  <si>
+    <t>Basim M</t>
+  </si>
+  <si>
+    <t>2025-04-07</t>
+  </si>
+  <si>
+    <t>Holistic Fitness 6kg Rubber Slam Ball</t>
+  </si>
+  <si>
+    <t>8,698</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>#FBZ-JLTUPXB</t>
   </si>
   <si>
     <t>Joyal Kuriakose</t>
   </si>
   <si>
-    <t>2025-02-04</t>
-  </si>
-  <si>
-    <t>Holistic Fitness 6kg Rubber Slam Ball</t>
-  </si>
-  <si>
-    <t>4,599</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>netbanking</t>
-  </si>
-  <si>
-    <t>Shipped</t>
-  </si>
-  <si>
-    <t>#FBZ-L1RGCSK</t>
-  </si>
-  <si>
-    <t>2025-01-04</t>
-  </si>
-  <si>
-    <t>MEDIX Soft Medicine Ball (2), Rubber for Adults</t>
-  </si>
-  <si>
-    <t>829</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>#FBZ-6C73256</t>
-  </si>
-  <si>
-    <t>Joyal K</t>
-  </si>
-  <si>
-    <t>2025-04-04</t>
-  </si>
-  <si>
-    <t>4,539</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>cod</t>
-  </si>
-  <si>
-    <t>Delivered</t>
-  </si>
-  <si>
-    <t>#FBZ-6C4S67Y</t>
-  </si>
-  <si>
-    <t>2025-03-04</t>
-  </si>
-  <si>
-    <t>769</t>
-  </si>
-  <si>
-    <t>#FBZ-QC1Q4GX</t>
-  </si>
-  <si>
-    <t>Abhinav K</t>
-  </si>
-  <si>
-    <t>Sports Premium Blitz Blue Kettlebell 8kg Cast Iron Vinyl Coated Solid Kettlebell</t>
-  </si>
-  <si>
-    <t>1,785</t>
-  </si>
-  <si>
-    <t>#FBZ-MO9A3PB</t>
-  </si>
-  <si>
-    <t>Twist Go Smart Watch for Men and Women</t>
-  </si>
-  <si>
-    <t>3,879</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>wallet</t>
-  </si>
-  <si>
-    <t>#FBZ-QUB1E3J</t>
-  </si>
-  <si>
-    <t>2025-04-03</t>
-  </si>
-  <si>
-    <t>Smart Health Wristband, Wearable Activity &amp; Fitness Tracker for Multi-Sport Mode</t>
-  </si>
-  <si>
-    <t>8,999</t>
-  </si>
-  <si>
-    <t>Out for Delivery</t>
-  </si>
-  <si>
-    <t>#FBZ-468CWKW</t>
-  </si>
-  <si>
-    <t>Achyuth J</t>
-  </si>
-  <si>
-    <t>Cast Iron Vinyl Coated Dumbbells for gym Workout</t>
-  </si>
-  <si>
-    <t>2,097</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>#FBZ-328BOQA</t>
-  </si>
-  <si>
-    <t>Achu K</t>
-  </si>
-  <si>
-    <t>2025-04-06</t>
-  </si>
-  <si>
-    <t>629</t>
-  </si>
-  <si>
-    <t>200</t>
+    <t>Adjustable Hand Grip Strengthener, Hand Gripper With Counter for Men</t>
+  </si>
+  <si>
+    <t>607</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>#FBZ-L0SXRRL</t>
+  </si>
+  <si>
+    <t>295</t>
   </si>
   <si>
     <t>Summary:</t>
@@ -196,19 +208,19 @@
     <t>Total Amount (₹)</t>
   </si>
   <si>
-    <t>₹28,125</t>
+    <t>₹16,588</t>
   </si>
   <si>
     <t>Total Discounts (₹)</t>
   </si>
   <si>
-    <t>₹740</t>
+    <t>₹1,525</t>
   </si>
   <si>
     <t>Net Sales (₹)</t>
   </si>
   <si>
-    <t>₹27,385</t>
+    <t>₹15,063</t>
   </si>
 </sst>
 </file>
@@ -709,22 +721,22 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,25 +747,25 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -764,31 +776,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -796,28 +808,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
         <v>17</v>
@@ -828,31 +840,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
         <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -860,31 +872,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -892,39 +904,39 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G12">
         <v>9</v>
@@ -932,35 +944,35 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final modifications and ui changes
</commit_message>
<xml_diff>
--- a/invoices/sales_report.xlsx
+++ b/invoices/sales_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
   <si>
     <t>SL No</t>
   </si>
@@ -43,22 +43,22 @@
     <t>Status</t>
   </si>
   <si>
-    <t>#FBZ-115EG1Y</t>
-  </si>
-  <si>
-    <t>Joyal K</t>
-  </si>
-  <si>
-    <t>2025-04-06</t>
-  </si>
-  <si>
-    <t>Kettle Bell 6 Kgs for home gym</t>
-  </si>
-  <si>
-    <t>1,008</t>
-  </si>
-  <si>
-    <t>150</t>
+    <t>#FBZ-VSBS9JH</t>
+  </si>
+  <si>
+    <t>Joyal Kuriakose</t>
+  </si>
+  <si>
+    <t>2025-04-11</t>
+  </si>
+  <si>
+    <t>Rubber Dumbbell Plates 30mm for Home or Professional Exercise Gym</t>
+  </si>
+  <si>
+    <t>4,320</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>netbanking</t>
@@ -67,133 +67,181 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>#FBZ-117E3WP</t>
-  </si>
-  <si>
-    <t>2025-04-05</t>
-  </si>
-  <si>
-    <t>Sports Premium Blitz Blue Kettlebell 8kg Cast Iron Vinyl Coated Solid Kettlebell</t>
-  </si>
-  <si>
-    <t>1,635</t>
+    <t>#FBZ-XVZN2K4</t>
+  </si>
+  <si>
+    <t>Adjustable Hand Grip Strengthener, Hand Gripper With Counter for Men</t>
+  </si>
+  <si>
+    <t>295</t>
+  </si>
+  <si>
+    <t>wallet</t>
+  </si>
+  <si>
+    <t>#FBZ-331FAVC</t>
+  </si>
+  <si>
+    <t>Achu K</t>
+  </si>
+  <si>
+    <t>MEDIX Soft Medicine Ball (2), Rubber for Adults</t>
+  </si>
+  <si>
+    <t>829</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>#FBZ-BSBADMH</t>
+  </si>
+  <si>
+    <t>2025-04-12</t>
+  </si>
+  <si>
+    <t>Returned</t>
+  </si>
+  <si>
+    <t>#FBZ-TT6Y9J9</t>
+  </si>
+  <si>
+    <t>Arundathi OA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Finger Gripper Strength Trainer | Hand Exerciser Yoga Resistance Bands</t>
+  </si>
+  <si>
+    <t>239</t>
+  </si>
+  <si>
+    <t>#FBZ-25VRN8N</t>
+  </si>
+  <si>
+    <t>Pair of two PVC Dumbbells Set Hex for all</t>
+  </si>
+  <si>
+    <t>1,065</t>
+  </si>
+  <si>
+    <t>#FBZ-DKTMF5O</t>
+  </si>
+  <si>
+    <t>Holistic Fitness 6kg Rubber Slam Ball</t>
+  </si>
+  <si>
+    <t>4,599</t>
+  </si>
+  <si>
+    <t>#FBZ-G3M74D5</t>
+  </si>
+  <si>
+    <t>#FBZ-GKKECKQ</t>
+  </si>
+  <si>
+    <t>1,039</t>
+  </si>
+  <si>
+    <t>#FBZ-HIETPNH</t>
+  </si>
+  <si>
+    <t>Twist Go Smart Watch for Men and Women</t>
+  </si>
+  <si>
+    <t>3,999</t>
+  </si>
+  <si>
+    <t>#FBZ-IVA9DSB</t>
+  </si>
+  <si>
+    <t>Smart Health Wristband, Wearable Activity &amp; Fitness Tracker for Multi-Sport Mode</t>
+  </si>
+  <si>
+    <t>8,999</t>
+  </si>
+  <si>
+    <t>#FBZ-29N17HT</t>
+  </si>
+  <si>
+    <t>Achyuth J</t>
+  </si>
+  <si>
+    <t>2025-04-13</t>
+  </si>
+  <si>
+    <t>Rubber Medicine Ball Weights for men &amp; women</t>
+  </si>
+  <si>
+    <t>2,177</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>#FBZ-O65P61O</t>
+  </si>
+  <si>
+    <t>Professional Gym Coated Solid Kettle Bells</t>
+  </si>
+  <si>
+    <t>1,839</t>
+  </si>
+  <si>
+    <t>#FBZ-SAPXLRA</t>
+  </si>
+  <si>
+    <t>#FBZ-19BPKKO</t>
+  </si>
+  <si>
+    <t>Professional Metal Integrted 5-40 Kg Spare Weight Plates Combo</t>
+  </si>
+  <si>
+    <t>1,514</t>
+  </si>
+  <si>
+    <t>#FBZ-S4C1VFT</t>
+  </si>
+  <si>
+    <t>Abhinav K</t>
+  </si>
+  <si>
+    <t>2025-04-14</t>
+  </si>
+  <si>
+    <t>3,799</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
   <si>
     <t>Delivered</t>
   </si>
   <si>
-    <t>#FBZ-PBMIZYX</t>
-  </si>
-  <si>
-    <t>Abhinav K</t>
-  </si>
-  <si>
-    <t>2025-04-04</t>
-  </si>
-  <si>
-    <t>Cast Iron Vinyl Coated Dumbbells for gym Workout</t>
-  </si>
-  <si>
-    <t>599</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>wallet</t>
-  </si>
-  <si>
-    <t>#FBZ-TM3CGR9</t>
-  </si>
-  <si>
-    <t>Cezanne P</t>
-  </si>
-  <si>
-    <t>2025-04-03</t>
-  </si>
-  <si>
-    <t>MEDIX Soft Medicine Ball (2), Rubber for Adults</t>
-  </si>
-  <si>
-    <t>629</t>
-  </si>
-  <si>
-    <t>#FBZ-VDGHF7G</t>
-  </si>
-  <si>
-    <t>Achyuth J</t>
-  </si>
-  <si>
-    <t>2025-04-02</t>
-  </si>
-  <si>
-    <t>Rubber Medicine Ball Weights for men &amp; women</t>
-  </si>
-  <si>
-    <t>2,052</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
-    <t>cod</t>
-  </si>
-  <si>
-    <t>#FBZ-XIPA8OQ</t>
-  </si>
-  <si>
-    <t>Achu K</t>
-  </si>
-  <si>
-    <t>2025-04-01</t>
-  </si>
-  <si>
-    <t>Pair of two PVC Dumbbells Set Hex for all</t>
-  </si>
-  <si>
-    <t>1,065</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>#FBZ-9VZ5PY4</t>
-  </si>
-  <si>
-    <t>Basim M</t>
-  </si>
-  <si>
-    <t>2025-04-07</t>
-  </si>
-  <si>
-    <t>Holistic Fitness 6kg Rubber Slam Ball</t>
-  </si>
-  <si>
-    <t>8,698</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>#FBZ-JLTUPXB</t>
-  </si>
-  <si>
-    <t>Joyal Kuriakose</t>
-  </si>
-  <si>
-    <t>Adjustable Hand Grip Strengthener, Hand Gripper With Counter for Men</t>
-  </si>
-  <si>
-    <t>607</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
-  </si>
-  <si>
-    <t>#FBZ-L0SXRRL</t>
-  </si>
-  <si>
-    <t>295</t>
+    <t>#FBZ-1PL0MPP</t>
+  </si>
+  <si>
+    <t>Yoga Mat</t>
+  </si>
+  <si>
+    <t>6,932</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>#FBZ-T9RYC2U</t>
+  </si>
+  <si>
+    <t>Rubber Coated Professional Exercise Hex Dumbbells (Pack Of 2)</t>
+  </si>
+  <si>
+    <t>1,960</t>
+  </si>
+  <si>
+    <t>#FBZ-FBJZWBV</t>
+  </si>
+  <si>
+    <t>Shipped</t>
   </si>
   <si>
     <t>Summary:</t>
@@ -208,19 +256,19 @@
     <t>Total Amount (₹)</t>
   </si>
   <si>
-    <t>₹16,588</t>
+    <t>₹44,617</t>
   </si>
   <si>
     <t>Total Discounts (₹)</t>
   </si>
   <si>
-    <t>₹1,525</t>
+    <t>₹466</t>
   </si>
   <si>
     <t>Net Sales (₹)</t>
   </si>
   <si>
-    <t>₹15,063</t>
+    <t>₹44,151</t>
   </si>
 </sst>
 </file>
@@ -597,7 +645,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J25"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -660,7 +708,7 @@
         <v>13</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -686,25 +734,25 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -712,28 +760,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
         <v>26</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -744,31 +792,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -776,28 +824,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
@@ -808,31 +856,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -840,31 +888,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -872,31 +920,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -904,75 +952,395 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
         <v>60</v>
       </c>
-      <c r="H10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
         <v>16</v>
       </c>
-      <c r="J10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="J16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="G12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C17" t="s">
         <v>63</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D17" t="s">
         <v>64</v>
       </c>
-      <c r="G13" t="s">
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="H17" t="s">
         <v>66</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="G15" t="s">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
         <v>69</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
making fully responsive working on admin side
</commit_message>
<xml_diff>
--- a/invoices/sales_report.xlsx
+++ b/invoices/sales_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="41">
   <si>
     <t>SL No</t>
   </si>
@@ -43,205 +43,79 @@
     <t>Status</t>
   </si>
   <si>
-    <t>#FBZ-VSBS9JH</t>
+    <t>#FZORD-70W02ZD</t>
+  </si>
+  <si>
+    <t>Abhinav K</t>
+  </si>
+  <si>
+    <t>2025-04-24</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>₹NaN</t>
+  </si>
+  <si>
+    <t>₹0</t>
+  </si>
+  <si>
+    <t>netbanking</t>
+  </si>
+  <si>
+    <t>#FZORD-B3U05MB</t>
+  </si>
+  <si>
+    <t>Cezanne P</t>
+  </si>
+  <si>
+    <t>#FZORD-FC2OCBX</t>
+  </si>
+  <si>
+    <t>Achu K</t>
+  </si>
+  <si>
+    <t>#FZORD-KF4NVIW</t>
+  </si>
+  <si>
+    <t>Achyuth J</t>
+  </si>
+  <si>
+    <t>wallet</t>
+  </si>
+  <si>
+    <t>#FZORD-N8ZCMLN</t>
   </si>
   <si>
     <t>Joyal Kuriakose</t>
   </si>
   <si>
-    <t>2025-04-11</t>
-  </si>
-  <si>
-    <t>Rubber Dumbbell Plates 30mm for Home or Professional Exercise Gym</t>
-  </si>
-  <si>
-    <t>4,320</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>netbanking</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>#FBZ-XVZN2K4</t>
-  </si>
-  <si>
-    <t>Adjustable Hand Grip Strengthener, Hand Gripper With Counter for Men</t>
-  </si>
-  <si>
-    <t>295</t>
-  </si>
-  <si>
-    <t>wallet</t>
-  </si>
-  <si>
-    <t>#FBZ-331FAVC</t>
-  </si>
-  <si>
-    <t>Achu K</t>
-  </si>
-  <si>
-    <t>MEDIX Soft Medicine Ball (2), Rubber for Adults</t>
-  </si>
-  <si>
-    <t>829</t>
-  </si>
-  <si>
-    <t>cod</t>
-  </si>
-  <si>
-    <t>#FBZ-BSBADMH</t>
-  </si>
-  <si>
-    <t>2025-04-12</t>
-  </si>
-  <si>
-    <t>Returned</t>
-  </si>
-  <si>
-    <t>#FBZ-TT6Y9J9</t>
+    <t>#FZORD-POZ835X</t>
+  </si>
+  <si>
+    <t>#FZORD-Y5UYDZ1</t>
+  </si>
+  <si>
+    <t>#FZORD-2DHIF8V</t>
   </si>
   <si>
     <t>Arundathi OA</t>
   </si>
   <si>
-    <t xml:space="preserve"> Finger Gripper Strength Trainer | Hand Exerciser Yoga Resistance Bands</t>
-  </si>
-  <si>
-    <t>239</t>
-  </si>
-  <si>
-    <t>#FBZ-25VRN8N</t>
-  </si>
-  <si>
-    <t>Pair of two PVC Dumbbells Set Hex for all</t>
-  </si>
-  <si>
-    <t>1,065</t>
-  </si>
-  <si>
-    <t>#FBZ-DKTMF5O</t>
-  </si>
-  <si>
-    <t>Holistic Fitness 6kg Rubber Slam Ball</t>
-  </si>
-  <si>
-    <t>4,599</t>
-  </si>
-  <si>
-    <t>#FBZ-G3M74D5</t>
-  </si>
-  <si>
-    <t>#FBZ-GKKECKQ</t>
-  </si>
-  <si>
-    <t>1,039</t>
-  </si>
-  <si>
-    <t>#FBZ-HIETPNH</t>
-  </si>
-  <si>
-    <t>Twist Go Smart Watch for Men and Women</t>
-  </si>
-  <si>
-    <t>3,999</t>
-  </si>
-  <si>
-    <t>#FBZ-IVA9DSB</t>
-  </si>
-  <si>
-    <t>Smart Health Wristband, Wearable Activity &amp; Fitness Tracker for Multi-Sport Mode</t>
-  </si>
-  <si>
-    <t>8,999</t>
-  </si>
-  <si>
-    <t>#FBZ-29N17HT</t>
-  </si>
-  <si>
-    <t>Achyuth J</t>
-  </si>
-  <si>
-    <t>2025-04-13</t>
-  </si>
-  <si>
-    <t>Rubber Medicine Ball Weights for men &amp; women</t>
-  </si>
-  <si>
-    <t>2,177</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
-  </si>
-  <si>
-    <t>#FBZ-O65P61O</t>
-  </si>
-  <si>
-    <t>Professional Gym Coated Solid Kettle Bells</t>
-  </si>
-  <si>
-    <t>1,839</t>
-  </si>
-  <si>
-    <t>#FBZ-SAPXLRA</t>
-  </si>
-  <si>
-    <t>#FBZ-19BPKKO</t>
-  </si>
-  <si>
-    <t>Professional Metal Integrted 5-40 Kg Spare Weight Plates Combo</t>
-  </si>
-  <si>
-    <t>1,514</t>
-  </si>
-  <si>
-    <t>#FBZ-S4C1VFT</t>
-  </si>
-  <si>
-    <t>Abhinav K</t>
-  </si>
-  <si>
-    <t>2025-04-14</t>
-  </si>
-  <si>
-    <t>3,799</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>Delivered</t>
-  </si>
-  <si>
-    <t>#FBZ-1PL0MPP</t>
-  </si>
-  <si>
-    <t>Yoga Mat</t>
-  </si>
-  <si>
-    <t>6,932</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>#FBZ-T9RYC2U</t>
-  </si>
-  <si>
-    <t>Rubber Coated Professional Exercise Hex Dumbbells (Pack Of 2)</t>
-  </si>
-  <si>
-    <t>1,960</t>
-  </si>
-  <si>
-    <t>#FBZ-FBJZWBV</t>
-  </si>
-  <si>
-    <t>Shipped</t>
+    <t>#FZORD-FOX5VDE</t>
+  </si>
+  <si>
+    <t>Basim M</t>
+  </si>
+  <si>
+    <t>#FZORD-M7AK3HD</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>#FZORD-MO2Q2O2</t>
   </si>
   <si>
     <t>Summary:</t>
@@ -256,19 +130,10 @@
     <t>Total Amount (₹)</t>
   </si>
   <si>
-    <t>₹44,617</t>
-  </si>
-  <si>
     <t>Total Discounts (₹)</t>
   </si>
   <si>
-    <t>₹466</t>
-  </si>
-  <si>
     <t>Net Sales (₹)</t>
-  </si>
-  <si>
-    <t>₹44,151</t>
   </si>
 </sst>
 </file>
@@ -645,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J20"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -691,7 +556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -708,7 +573,7 @@
         <v>13</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -719,16 +584,13 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -737,173 +599,158 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -911,127 +758,115 @@
       <c r="I8" t="s">
         <v>16</v>
       </c>
-      <c r="J8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -1039,31 +874,28 @@
       <c r="I12" t="s">
         <v>16</v>
       </c>
-      <c r="J12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -1071,276 +903,107 @@
       <c r="I13" t="s">
         <v>16</v>
       </c>
-      <c r="J13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
       </c>
       <c r="I14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
         <v>16</v>
       </c>
-      <c r="J14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="G17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" t="s">
-        <v>71</v>
-      </c>
-      <c r="I18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" t="s">
-        <v>84</v>
-      </c>
-      <c r="G25" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after all updates before hosting
</commit_message>
<xml_diff>
--- a/invoices/sales_report.xlsx
+++ b/invoices/sales_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>SL No</t>
   </si>
@@ -43,79 +43,64 @@
     <t>Status</t>
   </si>
   <si>
-    <t>#FZORD-70W02ZD</t>
-  </si>
-  <si>
-    <t>Abhinav K</t>
-  </si>
-  <si>
-    <t>2025-04-24</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>₹NaN</t>
+    <t>#FZORD-G700Q1N</t>
+  </si>
+  <si>
+    <t>Joyal Kuriakose</t>
+  </si>
+  <si>
+    <t>2025-04-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Finger Gripper Strength Trainer | Hand Exerciser Yoga Resistance Bands</t>
+  </si>
+  <si>
+    <t>₹400</t>
   </si>
   <si>
     <t>₹0</t>
   </si>
   <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>Placed</t>
+  </si>
+  <si>
+    <t>#FZORD-6W1TTB1</t>
+  </si>
+  <si>
+    <t>Iron Single Adjustable Dumbbells Set For Men &amp; Women</t>
+  </si>
+  <si>
+    <t>₹5,016</t>
+  </si>
+  <si>
+    <t>wallet</t>
+  </si>
+  <si>
+    <t>Shipped</t>
+  </si>
+  <si>
+    <t>Rubber Coated Professional Exercise Hex Dumbbells (Pack Of 2)</t>
+  </si>
+  <si>
+    <t>₹2,160</t>
+  </si>
+  <si>
+    <t>#FZORD-G28MSGL</t>
+  </si>
+  <si>
     <t>netbanking</t>
   </si>
   <si>
-    <t>#FZORD-B3U05MB</t>
-  </si>
-  <si>
-    <t>Cezanne P</t>
-  </si>
-  <si>
-    <t>#FZORD-FC2OCBX</t>
-  </si>
-  <si>
-    <t>Achu K</t>
-  </si>
-  <si>
-    <t>#FZORD-KF4NVIW</t>
-  </si>
-  <si>
-    <t>Achyuth J</t>
-  </si>
-  <si>
-    <t>wallet</t>
-  </si>
-  <si>
-    <t>#FZORD-N8ZCMLN</t>
-  </si>
-  <si>
-    <t>Joyal Kuriakose</t>
-  </si>
-  <si>
-    <t>#FZORD-POZ835X</t>
-  </si>
-  <si>
-    <t>#FZORD-Y5UYDZ1</t>
-  </si>
-  <si>
-    <t>#FZORD-2DHIF8V</t>
-  </si>
-  <si>
-    <t>Arundathi OA</t>
-  </si>
-  <si>
-    <t>#FZORD-FOX5VDE</t>
-  </si>
-  <si>
-    <t>Basim M</t>
-  </si>
-  <si>
-    <t>#FZORD-M7AK3HD</t>
-  </si>
-  <si>
-    <t>card</t>
-  </si>
-  <si>
-    <t>#FZORD-MO2Q2O2</t>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>#FZORD-JIYHT1Y</t>
+  </si>
+  <si>
+    <t>2025-04-28</t>
   </si>
   <si>
     <t>Summary:</t>
@@ -128,6 +113,9 @@
   </si>
   <si>
     <t>Total Amount (₹)</t>
+  </si>
+  <si>
+    <t>₹11,896</t>
   </si>
   <si>
     <t>Total Discounts (₹)</t>
@@ -510,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -556,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -573,7 +561,7 @@
         <v>13</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -584,13 +572,16 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -599,411 +590,162 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
         <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>